<commit_message>
emall edit of output table
</commit_message>
<xml_diff>
--- a/RAnalysis/Output/20191231_Stats_Day7_Day21.xlsx
+++ b/RAnalysis/Output/20191231_Stats_Day7_Day21.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\My_Projects\Inragenerational_thresholds_OA\RAnalysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EEF0F4-F5EA-4039-BDB2-5013F564B89B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43B5923-479D-4AF0-8110-7D899C27AC2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3FD9A52D-31BE-48B8-AD63-907FB3F60E42}"/>
   </bookViews>
   <sheets>
     <sheet name="Phys_Stats_Table" sheetId="1" r:id="rId1"/>
-    <sheet name="summary" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="summary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="109">
   <si>
     <t>Effect</t>
   </si>
@@ -2055,7 +2056,7 @@
   <dimension ref="B5:AF74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W50" sqref="W50"/>
+      <selection activeCell="B27" sqref="B27:J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3266,11 +3267,10 @@
       <c r="D34" s="48"/>
       <c r="E34" s="48"/>
       <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
+      <c r="G34" s="56" t="s">
+        <v>6</v>
+      </c>
       <c r="H34" s="56"/>
-      <c r="I34" s="56" t="s">
-        <v>6</v>
-      </c>
       <c r="J34" s="56"/>
       <c r="K34" s="48"/>
       <c r="L34" s="48"/>
@@ -3729,11 +3729,10 @@
       <c r="D44" s="48"/>
       <c r="E44" s="48"/>
       <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
+      <c r="G44" s="56" t="s">
+        <v>6</v>
+      </c>
       <c r="H44" s="56"/>
-      <c r="I44" s="56" t="s">
-        <v>6</v>
-      </c>
       <c r="J44" s="56"/>
       <c r="K44" s="48"/>
       <c r="L44" s="48"/>
@@ -4158,7 +4157,6 @@
       <c r="D53" s="45"/>
       <c r="E53" s="48"/>
       <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
       <c r="H53" s="48"/>
       <c r="I53" s="48"/>
       <c r="J53" s="48"/>
@@ -4191,11 +4189,10 @@
       <c r="D54" s="48"/>
       <c r="E54" s="48"/>
       <c r="F54" s="48"/>
-      <c r="G54" s="48"/>
+      <c r="G54" s="56" t="s">
+        <v>34</v>
+      </c>
       <c r="H54" s="56"/>
-      <c r="I54" s="56" t="s">
-        <v>34</v>
-      </c>
       <c r="J54" s="56"/>
       <c r="K54" s="48"/>
       <c r="L54" s="48"/>
@@ -4935,12 +4932,484 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D43:D45 H42 L42:L52 H53:L55 H52 K52 H70 H56 K56:L56 H57 K57:L57 H58 K58:L58 H59 J59:L59 H60 K60:L60 H61 K61:L61 H62 K62:L62 H63 K63:L63 H64 K64:L64 H65 K65:L65 H66 K66:L66 H67 K67:L67 H68 K68:L68 H69 K69:L69 K70:L70 D53:D55 D56:D70" numberStoredAsText="1"/>
+    <ignoredError sqref="D43:D45 H42 L42:L52 H53:L53 H52 K52 H70 H56 K56:L56 H57 K57:L57 H58 K58:L58 H59 J59:L59 H60 K60:L60 H61 K61:L61 H62 K62:L62 H63 K63:L63 H64 K64:L64 H65 K65:L65 H66 K66:L66 H67 K67:L67 H68 K68:L68 H69 K69:L69 K70:L70 D53:D55 D56:D70 H55:L55 H54 J54:L54" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE464377-C134-4C85-8895-E2C5B5E98A62}">
+  <dimension ref="B1:O18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" style="2" customWidth="1"/>
+    <col min="4" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="2" customWidth="1"/>
+    <col min="8" max="10" width="9.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="2" customWidth="1"/>
+    <col min="12" max="14" width="9.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="84"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="84"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="84"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+    </row>
+    <row r="6" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="3">
+        <v>9.3130000000000006</v>
+      </c>
+      <c r="N6" s="23">
+        <v>4.7299999999999998E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="3">
+        <v>2.536</v>
+      </c>
+      <c r="N7" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.377</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="3">
+        <v>2.1360000000000001</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.158</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.85463</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="60"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="45"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+    </row>
+    <row r="11" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8.0690000000000008</v>
+      </c>
+      <c r="F11" s="4">
+        <v>6.2700000000000004E-3</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.3650000000000002</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" s="2">
+        <v>12.898999999999999</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.84897999999999996</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1.5780000000000001</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.21534900000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2.161</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.14713999999999999</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1.272</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="2">
+        <v>3.298</v>
+      </c>
+      <c r="N13" s="24">
+        <v>7.4701000000000004E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.43</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.24796000000000001</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.423</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.756</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.18218599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.41363</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.50360000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.752</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.89063099999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="82">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="F17" s="19">
+        <v>0.86882000000000004</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="82">
+        <v>0.26</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="K17" s="19"/>
+      <c r="L17" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="19">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="N17" s="19">
+        <v>0.83532099999999998</v>
+      </c>
+      <c r="O17" s="19"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE01428-5470-4895-85FF-E357B31E924E}">
   <dimension ref="C1:P13"/>
   <sheetViews>

</xml_diff>

<commit_message>
small edit to italics in table
</commit_message>
<xml_diff>
--- a/RAnalysis/Output/20191231_Stats_Day7_Day21.xlsx
+++ b/RAnalysis/Output/20191231_Stats_Day7_Day21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\My_Projects\Inragenerational_thresholds_OA\RAnalysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43B5923-479D-4AF0-8110-7D899C27AC2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65210042-CE72-4CC6-AF71-3E92406A72CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3FD9A52D-31BE-48B8-AD63-907FB3F60E42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{3FD9A52D-31BE-48B8-AD63-907FB3F60E42}"/>
   </bookViews>
   <sheets>
     <sheet name="Phys_Stats_Table" sheetId="1" r:id="rId1"/>
@@ -1331,14 +1331,6 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1357,6 +1349,13 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1469,7 +1468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1554,26 +1553,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1628,16 +1627,13 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1678,17 +1674,23 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2055,7 +2057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E9823B-29CD-4BA3-B3B1-256E48CA27EB}">
   <dimension ref="B5:AF74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B27" sqref="B27:J72"/>
     </sheetView>
   </sheetViews>
@@ -2082,48 +2084,48 @@
       <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85" t="s">
+      <c r="C5" s="82"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="84"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="85" t="s">
+      <c r="F5" s="83"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="84"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="85" t="s">
+      <c r="J5" s="83"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="84"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="85" t="s">
+      <c r="N5" s="83"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="R5" s="84"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="84"/>
-      <c r="U5" s="85" t="s">
+      <c r="R5" s="83"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="84"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="18"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="85" t="s">
+      <c r="X5" s="83"/>
+      <c r="Y5" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="Z5" s="84"/>
-      <c r="AA5" s="86"/>
-      <c r="AB5" s="84"/>
-      <c r="AC5" s="85" t="s">
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="84"/>
+      <c r="AD5" s="83"/>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D6" s="21" t="s">
@@ -2441,7 +2443,7 @@
       <c r="AC11" s="3"/>
     </row>
     <row r="12" spans="2:32" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="80" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="60"/>
@@ -2476,34 +2478,34 @@
       <c r="AD12" s="45"/>
     </row>
     <row r="13" spans="2:32" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="82"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="81"/>
       <c r="R13" s="19"/>
       <c r="S13" s="19"/>
-      <c r="T13" s="82"/>
-      <c r="U13" s="82"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="81"/>
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
-      <c r="X13" s="82"/>
-      <c r="Y13" s="82"/>
+      <c r="X13" s="81"/>
+      <c r="Y13" s="81"/>
       <c r="Z13" s="19"/>
       <c r="AA13" s="19"/>
-      <c r="AB13" s="82"/>
-      <c r="AC13" s="82"/>
+      <c r="AB13" s="81"/>
+      <c r="AC13" s="81"/>
       <c r="AD13" s="19"/>
     </row>
     <row r="14" spans="2:32" ht="19.5" x14ac:dyDescent="0.35">
@@ -2879,51 +2881,51 @@
       <c r="AC19" s="3"/>
     </row>
     <row r="20" spans="2:32" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82" t="s">
+      <c r="C20" s="81"/>
+      <c r="D20" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="82">
+      <c r="E20" s="81">
         <v>0.36099999999999999</v>
       </c>
       <c r="F20" s="19">
         <v>0.69799999999999995</v>
       </c>
       <c r="G20" s="19"/>
-      <c r="H20" s="87">
+      <c r="H20" s="86">
         <v>2198</v>
       </c>
-      <c r="I20" s="82">
+      <c r="I20" s="81">
         <v>0.73</v>
       </c>
       <c r="J20" s="19">
         <v>0.48299999999999998</v>
       </c>
       <c r="K20" s="19"/>
-      <c r="L20" s="87">
+      <c r="L20" s="86">
         <v>2198</v>
       </c>
-      <c r="M20" s="82">
+      <c r="M20" s="81">
         <v>0.63100000000000001</v>
       </c>
-      <c r="N20" s="82">
+      <c r="N20" s="81">
         <v>0.53310000000000002</v>
       </c>
       <c r="O20" s="19"/>
-      <c r="P20" s="82" t="s">
+      <c r="P20" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="Q20" s="82">
+      <c r="Q20" s="81">
         <v>0.26</v>
       </c>
       <c r="R20" s="19">
         <v>0.77200000000000002</v>
       </c>
       <c r="S20" s="19"/>
-      <c r="T20" s="82" t="s">
+      <c r="T20" s="81" t="s">
         <v>76</v>
       </c>
       <c r="U20" s="19">
@@ -2933,18 +2935,18 @@
         <v>0.83532099999999998</v>
       </c>
       <c r="W20" s="19"/>
-      <c r="X20" s="82" t="s">
+      <c r="X20" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="Y20" s="82">
+      <c r="Y20" s="81">
         <v>0.14099999999999999</v>
       </c>
       <c r="Z20" s="19">
         <v>0.86882000000000004</v>
       </c>
       <c r="AA20" s="19"/>
-      <c r="AB20" s="82"/>
-      <c r="AC20" s="82"/>
+      <c r="AB20" s="81"/>
+      <c r="AC20" s="81"/>
       <c r="AD20" s="19"/>
     </row>
     <row r="21" spans="2:32" x14ac:dyDescent="0.25">
@@ -3042,26 +3044,26 @@
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="49"/>
-      <c r="E28" s="78" t="s">
+      <c r="E28" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="76"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="78" t="s">
+      <c r="F28" s="75"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="J28" s="76"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="78" t="s">
+      <c r="J28" s="75"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="N28" s="76"/>
+      <c r="N28" s="75"/>
     </row>
     <row r="29" spans="2:32" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="77"/>
-      <c r="C29" s="77"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
       <c r="D29" s="54" t="s">
         <v>10</v>
       </c>
@@ -3108,18 +3110,17 @@
       <c r="AD29" s="45"/>
     </row>
     <row r="30" spans="2:32" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="72" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
       <c r="E30" s="48"/>
       <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
+      <c r="G30" s="54" t="s">
+        <v>27</v>
+      </c>
       <c r="H30" s="56"/>
-      <c r="I30" s="54" t="s">
-        <v>27</v>
-      </c>
       <c r="J30" s="56"/>
       <c r="K30" s="48"/>
       <c r="L30" s="48"/>
@@ -3145,15 +3146,15 @@
       <c r="AF30" s="53"/>
     </row>
     <row r="31" spans="2:32" s="47" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="71"/>
+      <c r="B31" s="70"/>
       <c r="C31" s="49"/>
       <c r="D31" s="49"/>
       <c r="E31" s="49"/>
       <c r="F31" s="49"/>
       <c r="G31" s="49"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="72"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="71"/>
       <c r="K31" s="49"/>
       <c r="L31" s="49"/>
       <c r="M31" s="49"/>
@@ -3192,7 +3193,7 @@
         <v>0.55159999999999998</v>
       </c>
       <c r="G32" s="45"/>
-      <c r="H32" s="91">
+      <c r="H32" s="90">
         <v>2884</v>
       </c>
       <c r="I32" s="50" t="s">
@@ -3260,7 +3261,7 @@
       <c r="AD33" s="45"/>
     </row>
     <row r="34" spans="2:30" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="72" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="51"/>
@@ -3335,7 +3336,7 @@
       <c r="E36" s="62">
         <v>3.4089999999999998</v>
       </c>
-      <c r="F36" s="63">
+      <c r="F36" s="92">
         <v>6.8099999999999994E-2</v>
       </c>
       <c r="G36" s="48"/>
@@ -3345,7 +3346,7 @@
       <c r="I36" s="65">
         <v>3.4420000000000002</v>
       </c>
-      <c r="J36" s="66">
+      <c r="J36" s="91">
         <v>6.4500000000000002E-2</v>
       </c>
       <c r="K36" s="45"/>
@@ -3388,7 +3389,7 @@
       <c r="E37" s="62">
         <v>0.58399999999999996</v>
       </c>
-      <c r="F37" s="67">
+      <c r="F37" s="66">
         <v>0.55959999999999999</v>
       </c>
       <c r="G37" s="48"/>
@@ -3398,7 +3399,7 @@
       <c r="I37" s="65">
         <v>0.13700000000000001</v>
       </c>
-      <c r="J37" s="68">
+      <c r="J37" s="67">
         <v>0.87219999999999998</v>
       </c>
       <c r="K37" s="45"/>
@@ -3413,7 +3414,7 @@
       </c>
       <c r="O37" s="45"/>
       <c r="P37" s="45"/>
-      <c r="Q37" s="88" t="s">
+      <c r="Q37" s="87" t="s">
         <v>93</v>
       </c>
       <c r="R37" s="45"/>
@@ -3441,7 +3442,7 @@
       <c r="E38" s="62">
         <v>1.45</v>
       </c>
-      <c r="F38" s="67">
+      <c r="F38" s="66">
         <v>0.24</v>
       </c>
       <c r="G38" s="48"/>
@@ -3451,7 +3452,7 @@
       <c r="I38" s="65">
         <v>3.4470000000000001</v>
       </c>
-      <c r="J38" s="69">
+      <c r="J38" s="68">
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="K38" s="45"/>
@@ -3466,7 +3467,7 @@
       </c>
       <c r="O38" s="45"/>
       <c r="P38" s="45"/>
-      <c r="Q38" s="88" t="s">
+      <c r="Q38" s="87" t="s">
         <v>94</v>
       </c>
       <c r="R38" s="45"/>
@@ -3504,7 +3505,7 @@
       <c r="I39" s="65">
         <v>0.23499999999999999</v>
       </c>
-      <c r="J39" s="68">
+      <c r="J39" s="67">
         <v>0.79090000000000005</v>
       </c>
       <c r="K39" s="45"/>
@@ -3546,7 +3547,7 @@
       <c r="E40" s="62">
         <v>1.155</v>
       </c>
-      <c r="F40" s="67">
+      <c r="F40" s="66">
         <v>0.31990000000000002</v>
       </c>
       <c r="G40" s="48"/>
@@ -3556,7 +3557,7 @@
       <c r="I40" s="65">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J40" s="68">
+      <c r="J40" s="67">
         <v>0.98219999999999996</v>
       </c>
       <c r="K40" s="45"/>
@@ -3571,7 +3572,7 @@
       </c>
       <c r="O40" s="45"/>
       <c r="P40" s="45"/>
-      <c r="Q40" s="88" t="s">
+      <c r="Q40" s="87" t="s">
         <v>86</v>
       </c>
       <c r="R40" s="45"/>
@@ -3599,7 +3600,7 @@
       <c r="E41" s="62">
         <v>1.486</v>
       </c>
-      <c r="F41" s="67">
+      <c r="F41" s="66">
         <v>0.21310000000000001</v>
       </c>
       <c r="G41" s="48"/>
@@ -3609,7 +3610,7 @@
       <c r="I41" s="65">
         <v>0.14499999999999999</v>
       </c>
-      <c r="J41" s="68">
+      <c r="J41" s="67">
         <v>0.96499999999999997</v>
       </c>
       <c r="K41" s="45"/>
@@ -3650,17 +3651,17 @@
       <c r="E42" s="62">
         <v>0.57299999999999995</v>
       </c>
-      <c r="F42" s="67">
+      <c r="F42" s="66">
         <v>0.68300000000000005</v>
       </c>
       <c r="G42" s="48"/>
       <c r="H42" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I42" s="68">
+      <c r="I42" s="67">
         <v>1.2869999999999999</v>
       </c>
-      <c r="J42" s="68">
+      <c r="J42" s="67">
         <v>0.27489999999999998</v>
       </c>
       <c r="K42" s="45"/>
@@ -3722,7 +3723,7 @@
       <c r="AD43" s="45"/>
     </row>
     <row r="44" spans="2:30" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="72" t="s">
         <v>32</v>
       </c>
       <c r="C44" s="48"/>
@@ -3797,17 +3798,17 @@
       <c r="E46" s="62">
         <v>0.14899999999999999</v>
       </c>
-      <c r="F46" s="67">
+      <c r="F46" s="66">
         <v>0.70069999999999999</v>
       </c>
       <c r="G46" s="48"/>
       <c r="H46" s="64">
         <v>1306</v>
       </c>
-      <c r="I46" s="89">
+      <c r="I46" s="88">
         <v>1.6519999999999999</v>
       </c>
-      <c r="J46" s="89">
+      <c r="J46" s="88">
         <v>0.19950000000000001</v>
       </c>
       <c r="K46" s="45"/>
@@ -3850,17 +3851,17 @@
       <c r="E47" s="62">
         <v>2.3279999999999998</v>
       </c>
-      <c r="F47" s="67">
+      <c r="F47" s="66">
         <v>0.10349999999999999</v>
       </c>
       <c r="G47" s="48"/>
       <c r="H47" s="64">
         <v>2306</v>
       </c>
-      <c r="I47" s="89">
+      <c r="I47" s="88">
         <v>0.64700000000000002</v>
       </c>
-      <c r="J47" s="89">
+      <c r="J47" s="88">
         <v>0.5242</v>
       </c>
       <c r="K47" s="45"/>
@@ -3903,17 +3904,17 @@
       <c r="E48" s="62">
         <v>3.7189999999999999</v>
       </c>
-      <c r="F48" s="70">
+      <c r="F48" s="69">
         <v>2.8199999999999999E-2</v>
       </c>
       <c r="G48" s="48"/>
       <c r="H48" s="64">
         <v>2306</v>
       </c>
-      <c r="I48" s="89">
+      <c r="I48" s="88">
         <v>6.673</v>
       </c>
-      <c r="J48" s="90">
+      <c r="J48" s="89">
         <v>1.5E-3</v>
       </c>
       <c r="K48" s="45"/>
@@ -3956,17 +3957,17 @@
       <c r="E49" s="62">
         <v>1.004</v>
       </c>
-      <c r="F49" s="67">
+      <c r="F49" s="66">
         <v>0.37069999999999997</v>
       </c>
       <c r="G49" s="48"/>
       <c r="H49" s="64">
         <v>2306</v>
       </c>
-      <c r="I49" s="89">
+      <c r="I49" s="88">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="J49" s="89">
+      <c r="J49" s="88">
         <v>0.95</v>
       </c>
       <c r="K49" s="45"/>
@@ -4009,17 +4010,17 @@
       <c r="E50" s="62">
         <v>1.127</v>
       </c>
-      <c r="F50" s="67">
+      <c r="F50" s="66">
         <v>0.32879999999999998</v>
       </c>
       <c r="G50" s="48"/>
       <c r="H50" s="64">
         <v>2306</v>
       </c>
-      <c r="I50" s="89">
+      <c r="I50" s="88">
         <v>0.54200000000000004</v>
       </c>
-      <c r="J50" s="89">
+      <c r="J50" s="88">
         <v>0.58209999999999995</v>
       </c>
       <c r="K50" s="45"/>
@@ -4060,17 +4061,17 @@
       <c r="E51" s="62">
         <v>1.325</v>
       </c>
-      <c r="F51" s="67">
+      <c r="F51" s="66">
         <v>0.26719999999999999</v>
       </c>
       <c r="G51" s="48"/>
       <c r="H51" s="64">
         <v>4306</v>
       </c>
-      <c r="I51" s="89">
+      <c r="I51" s="88">
         <v>0.82399999999999995</v>
       </c>
-      <c r="J51" s="89">
+      <c r="J51" s="88">
         <v>0.51049999999999995</v>
       </c>
       <c r="K51" s="45"/>
@@ -4111,17 +4112,17 @@
       <c r="E52" s="62">
         <v>0.59699999999999998</v>
       </c>
-      <c r="F52" s="67">
+      <c r="F52" s="66">
         <v>0.66569999999999996</v>
       </c>
       <c r="G52" s="48"/>
       <c r="H52" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I52" s="89">
+      <c r="I52" s="88">
         <v>0.35299999999999998</v>
       </c>
-      <c r="J52" s="89">
+      <c r="J52" s="88">
         <v>0.8417</v>
       </c>
       <c r="K52" s="45"/>
@@ -4182,7 +4183,7 @@
       <c r="AD53" s="45"/>
     </row>
     <row r="54" spans="2:30" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="73" t="s">
+      <c r="B54" s="72" t="s">
         <v>33</v>
       </c>
       <c r="C54" s="48"/>
@@ -4216,7 +4217,7 @@
       <c r="AD54" s="45"/>
     </row>
     <row r="55" spans="2:30" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="74"/>
+      <c r="B55" s="73"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
       <c r="E55" s="19"/>
@@ -4224,7 +4225,7 @@
       <c r="G55" s="19"/>
       <c r="H55" s="19"/>
       <c r="I55" s="19"/>
-      <c r="J55" s="75"/>
+      <c r="J55" s="74"/>
       <c r="K55" s="19"/>
       <c r="L55" s="19"/>
       <c r="M55" s="19"/>
@@ -4301,7 +4302,7 @@
       <c r="T57" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="U57" s="88" t="s">
+      <c r="U57" s="87" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4380,7 +4381,7 @@
       <c r="T59" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="U59" s="88" t="s">
+      <c r="U59" s="87" t="s">
         <v>83</v>
       </c>
     </row>
@@ -4416,7 +4417,7 @@
       <c r="N60" s="2">
         <v>0.23372999999999999</v>
       </c>
-      <c r="U60" s="88" t="s">
+      <c r="U60" s="87" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4452,7 +4453,7 @@
       <c r="N61" s="4">
         <v>4.81E-3</v>
       </c>
-      <c r="U61" s="88" t="s">
+      <c r="U61" s="87" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4488,7 +4489,7 @@
       <c r="N62" s="4">
         <v>2.5389999999999999E-2</v>
       </c>
-      <c r="U62" s="88" t="s">
+      <c r="U62" s="87" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4639,7 +4640,7 @@
       <c r="T66" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="U66" s="88" t="s">
+      <c r="U66" s="87" t="s">
         <v>91</v>
       </c>
     </row>
@@ -4677,7 +4678,7 @@
       <c r="O67" s="25"/>
       <c r="R67" s="25"/>
       <c r="S67" s="25"/>
-      <c r="U67" s="88" t="s">
+      <c r="U67" s="87" t="s">
         <v>90</v>
       </c>
       <c r="W67" s="25"/>
@@ -4724,7 +4725,7 @@
       <c r="O68" s="25"/>
       <c r="R68" s="25"/>
       <c r="S68" s="25"/>
-      <c r="U68" s="88" t="s">
+      <c r="U68" s="87" t="s">
         <v>89</v>
       </c>
       <c r="V68" s="25"/>
@@ -4773,7 +4774,7 @@
       <c r="R69" s="25"/>
       <c r="S69" s="25"/>
       <c r="T69" s="25"/>
-      <c r="U69" s="88" t="s">
+      <c r="U69" s="87" t="s">
         <v>88</v>
       </c>
       <c r="V69" s="25"/>
@@ -4941,8 +4942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE464377-C134-4C85-8895-E2C5B5E98A62}">
   <dimension ref="B1:O18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4965,23 +4966,23 @@
         <v>0</v>
       </c>
       <c r="C2" s="18"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="85" t="s">
+      <c r="D2" s="83"/>
+      <c r="E2" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="84"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85" t="s">
+      <c r="F2" s="83"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="85" t="s">
+      <c r="J2" s="83"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="84"/>
+      <c r="N2" s="83"/>
       <c r="O2" s="18"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -5137,7 +5138,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="80" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="60"/>
@@ -5156,17 +5157,17 @@
       <c r="O9" s="45"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
+      <c r="B10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
     </row>
@@ -5263,7 +5264,7 @@
       <c r="M13" s="2">
         <v>3.298</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="21">
         <v>7.4701000000000004E-2</v>
       </c>
     </row>
@@ -5364,30 +5365,30 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="D17" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="82">
+      <c r="E17" s="81">
         <v>0.14099999999999999</v>
       </c>
       <c r="F17" s="19">
         <v>0.86882000000000004</v>
       </c>
       <c r="G17" s="19"/>
-      <c r="H17" s="82" t="s">
+      <c r="H17" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="82">
+      <c r="I17" s="81">
         <v>0.26</v>
       </c>
       <c r="J17" s="19">
         <v>0.77200000000000002</v>
       </c>
       <c r="K17" s="19"/>
-      <c r="L17" s="82" t="s">
+      <c r="L17" s="81" t="s">
         <v>76</v>
       </c>
       <c r="M17" s="19">

</xml_diff>